<commit_message>
3D Completo en 4K
</commit_message>
<xml_diff>
--- a/reporte2_P21.xlsx
+++ b/reporte2_P21.xlsx
@@ -51,7 +51,7 @@
     <t>Magnum</t>
   </si>
   <si>
-    <t>Oporto</t>
+    <t>Jerez</t>
   </si>
   <si>
     <t>Doble Magnum</t>
@@ -60,10 +60,10 @@
     <t>Blanco</t>
   </si>
   <si>
-    <t>Imperial</t>
+    <t>Oporto</t>
   </si>
   <si>
-    <t>Jerez</t>
+    <t>Imperial</t>
   </si>
   <si>
     <t>Rosado</t>
@@ -584,10 +584,10 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -601,10 +601,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -630,16 +630,16 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -647,10 +647,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -670,22 +670,22 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -693,22 +693,22 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -716,10 +716,10 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -739,10 +739,10 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -762,16 +762,16 @@
     </row>
     <row r="16">
       <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -785,22 +785,22 @@
     </row>
     <row r="17">
       <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -808,16 +808,16 @@
     </row>
     <row r="18">
       <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -831,22 +831,22 @@
     </row>
     <row r="19">
       <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -854,10 +854,10 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -877,10 +877,10 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -889,10 +889,10 @@
         <v>8</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -900,10 +900,10 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -946,10 +946,10 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -958,10 +958,10 @@
         <v>8</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -969,10 +969,10 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -992,10 +992,10 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1015,10 +1015,10 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1038,10 +1038,10 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1061,10 +1061,10 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1073,10 +1073,10 @@
         <v>8</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1096,10 +1096,10 @@
         <v>8</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1119,10 +1119,10 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1188,10 +1188,10 @@
         <v>8</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1234,10 +1234,10 @@
         <v>8</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -1280,10 +1280,10 @@
         <v>8</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -1303,10 +1303,10 @@
         <v>8</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -1349,10 +1349,10 @@
         <v>8</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -1372,10 +1372,10 @@
         <v>8</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -1412,10 +1412,10 @@
         <v>7</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -1435,16 +1435,16 @@
         <v>7</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -1458,16 +1458,16 @@
         <v>7</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -1481,10 +1481,10 @@
         <v>7</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1504,16 +1504,16 @@
         <v>7</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -1527,10 +1527,10 @@
         <v>7</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -1550,10 +1550,10 @@
         <v>7</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E50">
         <v>2</v>
@@ -1573,10 +1573,10 @@
         <v>7</v>
       </c>
       <c r="C51">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1596,10 +1596,10 @@
         <v>7</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -1619,16 +1619,16 @@
         <v>7</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -1642,16 +1642,16 @@
         <v>7</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -1665,10 +1665,10 @@
         <v>7</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -1688,16 +1688,16 @@
         <v>7</v>
       </c>
       <c r="C56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -1711,10 +1711,10 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -1734,10 +1734,10 @@
         <v>7</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -1757,16 +1757,16 @@
         <v>7</v>
       </c>
       <c r="C59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -1780,10 +1780,10 @@
         <v>7</v>
       </c>
       <c r="C60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -1803,16 +1803,16 @@
         <v>7</v>
       </c>
       <c r="C61">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -1820,16 +1820,16 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -1843,16 +1843,16 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -1866,16 +1866,16 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -1889,22 +1889,22 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G65">
         <v>1</v>
@@ -1912,16 +1912,16 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -1941,16 +1941,16 @@
         <v>7</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -1964,16 +1964,16 @@
         <v>7</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D68" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -1981,10 +1981,10 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -2004,10 +2004,10 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -2016,10 +2016,10 @@
         <v>8</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G70">
         <v>1</v>
@@ -2027,10 +2027,10 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2073,10 +2073,10 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2096,10 +2096,10 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2200,10 +2200,10 @@
         <v>8</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G78">
         <v>1</v>
@@ -2269,10 +2269,10 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -2292,10 +2292,10 @@
         <v>8</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -2315,10 +2315,10 @@
         <v>8</v>
       </c>
       <c r="E83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G83">
         <v>1</v>
@@ -2338,10 +2338,10 @@
         <v>8</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -2361,10 +2361,10 @@
         <v>8</v>
       </c>
       <c r="E85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G85">
         <v>1</v>
@@ -2384,10 +2384,10 @@
         <v>8</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G86">
         <v>1</v>
@@ -2407,10 +2407,10 @@
         <v>8</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G87">
         <v>1</v>
@@ -2499,10 +2499,10 @@
         <v>8</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -2591,10 +2591,10 @@
         <v>8</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -2637,10 +2637,10 @@
         <v>8</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G97">
         <v>1</v>
@@ -2683,10 +2683,10 @@
         <v>8</v>
       </c>
       <c r="E99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G99">
         <v>1</v>
@@ -2706,10 +2706,10 @@
         <v>8</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -2729,10 +2729,10 @@
         <v>8</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -2740,10 +2740,10 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -2763,10 +2763,10 @@
     </row>
     <row r="103">
       <c r="A103">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -2786,10 +2786,10 @@
     </row>
     <row r="104">
       <c r="A104">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -2809,10 +2809,10 @@
     </row>
     <row r="105">
       <c r="A105">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -2821,10 +2821,10 @@
         <v>8</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G105">
         <v>1</v>
@@ -2835,7 +2835,7 @@
         <v>3</v>
       </c>
       <c r="B106" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -2858,7 +2858,7 @@
         <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -2867,10 +2867,10 @@
         <v>8</v>
       </c>
       <c r="E107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G107">
         <v>1</v>
@@ -2881,7 +2881,7 @@
         <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -2890,10 +2890,10 @@
         <v>8</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G108">
         <v>1</v>
@@ -2904,7 +2904,7 @@
         <v>3</v>
       </c>
       <c r="B109" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -2927,7 +2927,7 @@
         <v>3</v>
       </c>
       <c r="B110" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -2950,7 +2950,7 @@
         <v>3</v>
       </c>
       <c r="B111" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -2959,10 +2959,10 @@
         <v>8</v>
       </c>
       <c r="E111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F111" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G111">
         <v>1</v>
@@ -2973,7 +2973,7 @@
         <v>3</v>
       </c>
       <c r="B112" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -2982,10 +2982,10 @@
         <v>8</v>
       </c>
       <c r="E112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F112" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G112">
         <v>1</v>
@@ -2996,7 +2996,7 @@
         <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -3005,10 +3005,10 @@
         <v>8</v>
       </c>
       <c r="E113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F113" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G113">
         <v>1</v>
@@ -3019,7 +3019,7 @@
         <v>3</v>
       </c>
       <c r="B114" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -3042,7 +3042,7 @@
         <v>3</v>
       </c>
       <c r="B115" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -3062,10 +3062,10 @@
     </row>
     <row r="116">
       <c r="A116">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B116" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -3074,10 +3074,10 @@
         <v>8</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G116">
         <v>1</v>
@@ -3085,10 +3085,10 @@
     </row>
     <row r="117">
       <c r="A117">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B117" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -3108,10 +3108,10 @@
     </row>
     <row r="118">
       <c r="A118">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B118" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -3131,10 +3131,10 @@
     </row>
     <row r="119">
       <c r="A119">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B119" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -3143,10 +3143,10 @@
         <v>8</v>
       </c>
       <c r="E119">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F119" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G119">
         <v>1</v>
@@ -3154,10 +3154,10 @@
     </row>
     <row r="120">
       <c r="A120">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B120" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -3166,10 +3166,10 @@
         <v>8</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F120" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G120">
         <v>1</v>
@@ -3177,10 +3177,10 @@
     </row>
     <row r="121">
       <c r="A121">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -3200,10 +3200,10 @@
     </row>
     <row r="122">
       <c r="A122">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B122" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -3223,10 +3223,10 @@
     </row>
     <row r="123">
       <c r="A123">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B123" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -3246,10 +3246,10 @@
     </row>
     <row r="124">
       <c r="A124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B124" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -3269,10 +3269,10 @@
     </row>
     <row r="125">
       <c r="A125">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B125" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -3281,10 +3281,10 @@
         <v>8</v>
       </c>
       <c r="E125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F125" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G125">
         <v>1</v>
@@ -3292,10 +3292,10 @@
     </row>
     <row r="126">
       <c r="A126">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B126" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -3315,10 +3315,10 @@
     </row>
     <row r="127">
       <c r="A127">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B127" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -3327,10 +3327,10 @@
         <v>8</v>
       </c>
       <c r="E127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F127" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G127">
         <v>1</v>
@@ -3338,10 +3338,10 @@
     </row>
     <row r="128">
       <c r="A128">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B128" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -3350,10 +3350,10 @@
         <v>8</v>
       </c>
       <c r="E128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F128" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G128">
         <v>1</v>
@@ -3361,10 +3361,10 @@
     </row>
     <row r="129">
       <c r="A129">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B129" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -3384,10 +3384,10 @@
     </row>
     <row r="130">
       <c r="A130">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B130" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -3407,10 +3407,10 @@
     </row>
     <row r="131">
       <c r="A131">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B131" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -3430,10 +3430,10 @@
     </row>
     <row r="132">
       <c r="A132">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B132" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -3442,10 +3442,10 @@
         <v>8</v>
       </c>
       <c r="E132">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F132" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G132">
         <v>1</v>
@@ -3453,10 +3453,10 @@
     </row>
     <row r="133">
       <c r="A133">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -3465,10 +3465,10 @@
         <v>8</v>
       </c>
       <c r="E133">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F133" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G133">
         <v>1</v>
@@ -3476,10 +3476,10 @@
     </row>
     <row r="134">
       <c r="A134">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -3499,10 +3499,10 @@
     </row>
     <row r="135">
       <c r="A135">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B135" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -3522,10 +3522,10 @@
     </row>
     <row r="136">
       <c r="A136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B136" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -3545,10 +3545,10 @@
     </row>
     <row r="137">
       <c r="A137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B137" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -3568,10 +3568,10 @@
     </row>
     <row r="138">
       <c r="A138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B138" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -3580,10 +3580,10 @@
         <v>8</v>
       </c>
       <c r="E138">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F138" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G138">
         <v>1</v>
@@ -3591,10 +3591,10 @@
     </row>
     <row r="139">
       <c r="A139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B139" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -3614,10 +3614,10 @@
     </row>
     <row r="140">
       <c r="A140">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B140" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -3637,10 +3637,10 @@
     </row>
     <row r="141">
       <c r="A141">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B141" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -3649,10 +3649,10 @@
         <v>8</v>
       </c>
       <c r="E141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F141" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G141">
         <v>1</v>
@@ -3660,10 +3660,10 @@
     </row>
     <row r="142">
       <c r="A142">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B142" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -3672,10 +3672,10 @@
         <v>8</v>
       </c>
       <c r="E142">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F142" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G142">
         <v>1</v>
@@ -3683,10 +3683,10 @@
     </row>
     <row r="143">
       <c r="A143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B143" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -3706,10 +3706,10 @@
     </row>
     <row r="144">
       <c r="A144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B144" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -3718,10 +3718,10 @@
         <v>8</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F144" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G144">
         <v>1</v>
@@ -3729,10 +3729,10 @@
     </row>
     <row r="145">
       <c r="A145">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B145" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -3741,10 +3741,10 @@
         <v>8</v>
       </c>
       <c r="E145">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F145" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G145">
         <v>1</v>
@@ -3752,10 +3752,10 @@
     </row>
     <row r="146">
       <c r="A146">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B146" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -3764,10 +3764,10 @@
         <v>8</v>
       </c>
       <c r="E146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F146" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G146">
         <v>1</v>
@@ -3775,10 +3775,10 @@
     </row>
     <row r="147">
       <c r="A147">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B147" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -3798,10 +3798,10 @@
     </row>
     <row r="148">
       <c r="A148">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B148" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -3810,10 +3810,10 @@
         <v>8</v>
       </c>
       <c r="E148">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F148" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G148">
         <v>1</v>
@@ -3821,10 +3821,10 @@
     </row>
     <row r="149">
       <c r="A149">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -3844,10 +3844,10 @@
     </row>
     <row r="150">
       <c r="A150">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B150" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -3879,10 +3879,10 @@
         <v>8</v>
       </c>
       <c r="E151">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F151" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G151">
         <v>1</v>
@@ -3902,10 +3902,10 @@
         <v>8</v>
       </c>
       <c r="E152">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F152" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G152">
         <v>1</v>
@@ -3959,10 +3959,10 @@
     </row>
     <row r="155">
       <c r="A155">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -3982,10 +3982,10 @@
     </row>
     <row r="156">
       <c r="A156">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B156" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -3994,10 +3994,10 @@
         <v>8</v>
       </c>
       <c r="E156">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F156" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G156">
         <v>1</v>
@@ -4005,10 +4005,10 @@
     </row>
     <row r="157">
       <c r="A157">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B157" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -4028,10 +4028,10 @@
     </row>
     <row r="158">
       <c r="A158">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -4051,10 +4051,10 @@
     </row>
     <row r="159">
       <c r="A159">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B159" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -4074,10 +4074,10 @@
     </row>
     <row r="160">
       <c r="A160">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B160" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -4097,10 +4097,10 @@
     </row>
     <row r="161">
       <c r="A161">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B161" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -4120,10 +4120,10 @@
     </row>
     <row r="162">
       <c r="A162">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B162" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C162">
         <v>1</v>
@@ -4143,10 +4143,10 @@
     </row>
     <row r="163">
       <c r="A163">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B163" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -4155,10 +4155,10 @@
         <v>8</v>
       </c>
       <c r="E163">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F163" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G163">
         <v>1</v>
@@ -4178,10 +4178,10 @@
         <v>8</v>
       </c>
       <c r="E164">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F164" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G164">
         <v>1</v>
@@ -4201,10 +4201,10 @@
         <v>8</v>
       </c>
       <c r="E165">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F165" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G165">
         <v>1</v>
@@ -4241,10 +4241,10 @@
         <v>7</v>
       </c>
       <c r="C167">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D167" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E167">
         <v>1</v>
@@ -4264,16 +4264,16 @@
         <v>7</v>
       </c>
       <c r="C168">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D168" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E168">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F168" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G168">
         <v>1</v>
@@ -4287,16 +4287,16 @@
         <v>7</v>
       </c>
       <c r="C169">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D169" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E169">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F169" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G169">
         <v>1</v>
@@ -4310,10 +4310,10 @@
         <v>7</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D170" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E170">
         <v>1</v>
@@ -4333,10 +4333,10 @@
         <v>7</v>
       </c>
       <c r="C171">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D171" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -4356,10 +4356,10 @@
         <v>7</v>
       </c>
       <c r="C172">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D172" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E172">
         <v>1</v>
@@ -4379,10 +4379,10 @@
         <v>7</v>
       </c>
       <c r="C173">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D173" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E173">
         <v>1</v>
@@ -4402,16 +4402,16 @@
         <v>7</v>
       </c>
       <c r="C174">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E174">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F174" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G174">
         <v>1</v>
@@ -4523,10 +4523,10 @@
         <v>8</v>
       </c>
       <c r="E179">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F179" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G179">
         <v>1</v>
@@ -4592,10 +4592,10 @@
         <v>8</v>
       </c>
       <c r="E182">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F182" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G182">
         <v>1</v>
@@ -4615,10 +4615,10 @@
         <v>8</v>
       </c>
       <c r="E183">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F183" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G183">
         <v>1</v>
@@ -4701,10 +4701,10 @@
         <v>14</v>
       </c>
       <c r="C187">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D187" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E187">
         <v>2</v>
@@ -4724,10 +4724,10 @@
         <v>14</v>
       </c>
       <c r="C188">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D188" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -4822,10 +4822,10 @@
         <v>8</v>
       </c>
       <c r="E192">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F192" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G192">
         <v>1</v>
@@ -4914,10 +4914,10 @@
         <v>8</v>
       </c>
       <c r="E196">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F196" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G196">
         <v>1</v>
@@ -4960,10 +4960,10 @@
         <v>8</v>
       </c>
       <c r="E198">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F198" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G198">
         <v>1</v>
@@ -4983,10 +4983,10 @@
         <v>8</v>
       </c>
       <c r="E199">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F199" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G199">
         <v>1</v>
@@ -5006,10 +5006,10 @@
         <v>8</v>
       </c>
       <c r="E200">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F200" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G200">
         <v>1</v>
@@ -5017,10 +5017,10 @@
     </row>
     <row r="201">
       <c r="A201">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B201" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -5040,10 +5040,10 @@
     </row>
     <row r="202">
       <c r="A202">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B202" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -5063,10 +5063,10 @@
     </row>
     <row r="203">
       <c r="A203">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B203" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C203">
         <v>1</v>
@@ -5075,10 +5075,10 @@
         <v>8</v>
       </c>
       <c r="E203">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F203" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G203">
         <v>1</v>
@@ -5086,10 +5086,10 @@
     </row>
     <row r="204">
       <c r="A204">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B204" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -5098,10 +5098,10 @@
         <v>8</v>
       </c>
       <c r="E204">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F204" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G204">
         <v>1</v>
@@ -5109,10 +5109,10 @@
     </row>
     <row r="205">
       <c r="A205">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B205" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -5132,10 +5132,10 @@
     </row>
     <row r="206">
       <c r="A206">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B206" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -5155,10 +5155,10 @@
     </row>
     <row r="207">
       <c r="A207">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B207" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -5178,10 +5178,10 @@
     </row>
     <row r="208">
       <c r="A208">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B208" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -5190,10 +5190,10 @@
         <v>8</v>
       </c>
       <c r="E208">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F208" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G208">
         <v>1</v>
@@ -5201,10 +5201,10 @@
     </row>
     <row r="209">
       <c r="A209">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B209" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C209">
         <v>1</v>
@@ -5213,10 +5213,10 @@
         <v>8</v>
       </c>
       <c r="E209">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F209" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G209">
         <v>1</v>
@@ -5224,10 +5224,10 @@
     </row>
     <row r="210">
       <c r="A210">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B210" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C210">
         <v>1</v>
@@ -5247,10 +5247,10 @@
     </row>
     <row r="211">
       <c r="A211">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B211" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C211">
         <v>1</v>
@@ -5270,10 +5270,10 @@
     </row>
     <row r="212">
       <c r="A212">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B212" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C212">
         <v>1</v>
@@ -5293,22 +5293,22 @@
     </row>
     <row r="213">
       <c r="A213">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B213" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C213">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D213" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E213">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F213" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G213">
         <v>1</v>
@@ -5316,22 +5316,22 @@
     </row>
     <row r="214">
       <c r="A214">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B214" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C214">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D214" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E214">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F214" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G214">
         <v>1</v>
@@ -5339,10 +5339,10 @@
     </row>
     <row r="215">
       <c r="A215">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B215" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C215">
         <v>2</v>
@@ -5362,10 +5362,10 @@
     </row>
     <row r="216">
       <c r="A216">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B216" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C216">
         <v>2</v>
@@ -5385,10 +5385,10 @@
     </row>
     <row r="217">
       <c r="A217">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B217" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C217">
         <v>2</v>
@@ -5397,10 +5397,10 @@
         <v>11</v>
       </c>
       <c r="E217">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F217" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G217">
         <v>1</v>
@@ -5408,10 +5408,10 @@
     </row>
     <row r="218">
       <c r="A218">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B218" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C218">
         <v>2</v>
@@ -5420,10 +5420,10 @@
         <v>11</v>
       </c>
       <c r="E218">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F218" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G218">
         <v>1</v>
@@ -5431,10 +5431,10 @@
     </row>
     <row r="219">
       <c r="A219">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B219" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C219">
         <v>2</v>
@@ -5443,10 +5443,10 @@
         <v>11</v>
       </c>
       <c r="E219">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F219" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G219">
         <v>1</v>
@@ -5454,10 +5454,10 @@
     </row>
     <row r="220">
       <c r="A220">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B220" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C220">
         <v>2</v>
@@ -5480,19 +5480,19 @@
         <v>3</v>
       </c>
       <c r="B221" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C221">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D221" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E221">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F221" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G221">
         <v>1</v>
@@ -5500,10 +5500,10 @@
     </row>
     <row r="222">
       <c r="A222">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B222" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -5512,10 +5512,10 @@
         <v>8</v>
       </c>
       <c r="E222">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F222" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G222">
         <v>1</v>
@@ -5523,10 +5523,10 @@
     </row>
     <row r="223">
       <c r="A223">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B223" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -5535,10 +5535,10 @@
         <v>8</v>
       </c>
       <c r="E223">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F223" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G223">
         <v>1</v>
@@ -5546,10 +5546,10 @@
     </row>
     <row r="224">
       <c r="A224">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B224" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -5558,10 +5558,10 @@
         <v>8</v>
       </c>
       <c r="E224">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F224" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G224">
         <v>1</v>
@@ -5569,10 +5569,10 @@
     </row>
     <row r="225">
       <c r="A225">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B225" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -5581,10 +5581,10 @@
         <v>8</v>
       </c>
       <c r="E225">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F225" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G225">
         <v>1</v>
@@ -5592,10 +5592,10 @@
     </row>
     <row r="226">
       <c r="A226">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B226" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -5615,10 +5615,10 @@
     </row>
     <row r="227">
       <c r="A227">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B227" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C227">
         <v>1</v>
@@ -5627,10 +5627,10 @@
         <v>8</v>
       </c>
       <c r="E227">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F227" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G227">
         <v>1</v>
@@ -5638,10 +5638,10 @@
     </row>
     <row r="228">
       <c r="A228">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B228" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -5650,10 +5650,10 @@
         <v>8</v>
       </c>
       <c r="E228">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F228" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G228">
         <v>1</v>
@@ -5661,10 +5661,10 @@
     </row>
     <row r="229">
       <c r="A229">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B229" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -5684,10 +5684,10 @@
     </row>
     <row r="230">
       <c r="A230">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B230" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C230">
         <v>1</v>
@@ -5707,22 +5707,22 @@
     </row>
     <row r="231">
       <c r="A231">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B231" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C231">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D231" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E231">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F231" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G231">
         <v>1</v>
@@ -5730,16 +5730,16 @@
     </row>
     <row r="232">
       <c r="A232">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B232" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C232">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D232" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -5753,10 +5753,10 @@
     </row>
     <row r="233">
       <c r="A233">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B233" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C233">
         <v>2</v>
@@ -5765,10 +5765,10 @@
         <v>11</v>
       </c>
       <c r="E233">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F233" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G233">
         <v>1</v>
@@ -5776,22 +5776,22 @@
     </row>
     <row r="234">
       <c r="A234">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B234" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C234">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D234" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E234">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F234" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G234">
         <v>1</v>
@@ -5799,22 +5799,22 @@
     </row>
     <row r="235">
       <c r="A235">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B235" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D235" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E235">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F235" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G235">
         <v>1</v>
@@ -5822,16 +5822,16 @@
     </row>
     <row r="236">
       <c r="A236">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B236" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C236">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D236" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E236">
         <v>1</v>
@@ -5845,16 +5845,16 @@
     </row>
     <row r="237">
       <c r="A237">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B237" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C237">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D237" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E237">
         <v>1</v>
@@ -5868,16 +5868,16 @@
     </row>
     <row r="238">
       <c r="A238">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B238" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C238">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D238" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E238">
         <v>1</v>
@@ -5891,10 +5891,10 @@
     </row>
     <row r="239">
       <c r="A239">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B239" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C239">
         <v>2</v>
@@ -5903,10 +5903,10 @@
         <v>11</v>
       </c>
       <c r="E239">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F239" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G239">
         <v>1</v>
@@ -5914,24 +5914,300 @@
     </row>
     <row r="240">
       <c r="A240">
+        <v>4</v>
+      </c>
+      <c r="B240" t="s">
+        <v>12</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240" t="s">
+        <v>8</v>
+      </c>
+      <c r="E240">
+        <v>1</v>
+      </c>
+      <c r="F240" t="s">
+        <v>10</v>
+      </c>
+      <c r="G240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241">
+        <v>4</v>
+      </c>
+      <c r="B241" t="s">
+        <v>12</v>
+      </c>
+      <c r="C241">
+        <v>1</v>
+      </c>
+      <c r="D241" t="s">
+        <v>8</v>
+      </c>
+      <c r="E241">
+        <v>1</v>
+      </c>
+      <c r="F241" t="s">
+        <v>10</v>
+      </c>
+      <c r="G241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242">
+        <v>4</v>
+      </c>
+      <c r="B242" t="s">
+        <v>12</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+      <c r="D242" t="s">
+        <v>8</v>
+      </c>
+      <c r="E242">
+        <v>1</v>
+      </c>
+      <c r="F242" t="s">
+        <v>10</v>
+      </c>
+      <c r="G242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243">
+        <v>4</v>
+      </c>
+      <c r="B243" t="s">
+        <v>12</v>
+      </c>
+      <c r="C243">
+        <v>2</v>
+      </c>
+      <c r="D243" t="s">
+        <v>11</v>
+      </c>
+      <c r="E243">
+        <v>1</v>
+      </c>
+      <c r="F243" t="s">
+        <v>10</v>
+      </c>
+      <c r="G243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244">
+        <v>4</v>
+      </c>
+      <c r="B244" t="s">
+        <v>12</v>
+      </c>
+      <c r="C244">
+        <v>2</v>
+      </c>
+      <c r="D244" t="s">
+        <v>11</v>
+      </c>
+      <c r="E244">
+        <v>2</v>
+      </c>
+      <c r="F244" t="s">
+        <v>9</v>
+      </c>
+      <c r="G244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245">
+        <v>4</v>
+      </c>
+      <c r="B245" t="s">
+        <v>12</v>
+      </c>
+      <c r="C245">
+        <v>2</v>
+      </c>
+      <c r="D245" t="s">
+        <v>11</v>
+      </c>
+      <c r="E245">
+        <v>2</v>
+      </c>
+      <c r="F245" t="s">
+        <v>9</v>
+      </c>
+      <c r="G245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246">
         <v>5</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B246" t="s">
         <v>17</v>
       </c>
-      <c r="C240">
-        <v>2</v>
-      </c>
-      <c r="D240" t="s">
+      <c r="C246">
+        <v>1</v>
+      </c>
+      <c r="D246" t="s">
+        <v>8</v>
+      </c>
+      <c r="E246">
+        <v>2</v>
+      </c>
+      <c r="F246" t="s">
+        <v>9</v>
+      </c>
+      <c r="G246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247">
+        <v>5</v>
+      </c>
+      <c r="B247" t="s">
+        <v>17</v>
+      </c>
+      <c r="C247">
+        <v>1</v>
+      </c>
+      <c r="D247" t="s">
+        <v>8</v>
+      </c>
+      <c r="E247">
+        <v>2</v>
+      </c>
+      <c r="F247" t="s">
+        <v>9</v>
+      </c>
+      <c r="G247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248">
+        <v>5</v>
+      </c>
+      <c r="B248" t="s">
+        <v>17</v>
+      </c>
+      <c r="C248">
+        <v>1</v>
+      </c>
+      <c r="D248" t="s">
+        <v>8</v>
+      </c>
+      <c r="E248">
+        <v>2</v>
+      </c>
+      <c r="F248" t="s">
+        <v>9</v>
+      </c>
+      <c r="G248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249">
+        <v>5</v>
+      </c>
+      <c r="B249" t="s">
+        <v>17</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+      <c r="D249" t="s">
+        <v>8</v>
+      </c>
+      <c r="E249">
+        <v>1</v>
+      </c>
+      <c r="F249" t="s">
+        <v>10</v>
+      </c>
+      <c r="G249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250">
+        <v>5</v>
+      </c>
+      <c r="B250" t="s">
+        <v>17</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250" t="s">
+        <v>8</v>
+      </c>
+      <c r="E250">
+        <v>1</v>
+      </c>
+      <c r="F250" t="s">
+        <v>10</v>
+      </c>
+      <c r="G250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251">
+        <v>5</v>
+      </c>
+      <c r="B251" t="s">
+        <v>17</v>
+      </c>
+      <c r="C251">
+        <v>2</v>
+      </c>
+      <c r="D251" t="s">
         <v>11</v>
       </c>
-      <c r="E240">
-        <v>2</v>
-      </c>
-      <c r="F240" t="s">
-        <v>9</v>
-      </c>
-      <c r="G240">
+      <c r="E251">
+        <v>1</v>
+      </c>
+      <c r="F251" t="s">
+        <v>10</v>
+      </c>
+      <c r="G251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252">
+        <v>5</v>
+      </c>
+      <c r="B252" t="s">
+        <v>17</v>
+      </c>
+      <c r="C252">
+        <v>2</v>
+      </c>
+      <c r="D252" t="s">
+        <v>11</v>
+      </c>
+      <c r="E252">
+        <v>1</v>
+      </c>
+      <c r="F252" t="s">
+        <v>10</v>
+      </c>
+      <c r="G252">
         <v>1</v>
       </c>
     </row>

</xml_diff>